<commit_message>
Change Time to Int values
</commit_message>
<xml_diff>
--- a/0_data/aDNA_30GPs_new_samples.xlsx
+++ b/0_data/aDNA_30GPs_new_samples.xlsx
@@ -8000,7 +8000,7 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>15458.5</v>
+        <v>15458</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -8129,7 +8129,7 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>15130.5</v>
+        <v>15130</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -8516,7 +8516,7 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>34844.5</v>
+        <v>34844</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -10064,7 +10064,7 @@
         </is>
       </c>
       <c r="D75" t="n">
-        <v>10841.5</v>
+        <v>10841</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -10193,7 +10193,7 @@
         </is>
       </c>
       <c r="D76" t="n">
-        <v>31006.5</v>
+        <v>31006</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -10322,7 +10322,7 @@
         </is>
       </c>
       <c r="D77" t="n">
-        <v>30977.5</v>
+        <v>30977</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -10451,7 +10451,7 @@
         </is>
       </c>
       <c r="D78" t="n">
-        <v>10124.5</v>
+        <v>10124</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -10967,7 +10967,7 @@
         </is>
       </c>
       <c r="D82" t="n">
-        <v>8300.5</v>
+        <v>8300</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -11096,7 +11096,7 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>8864.5</v>
+        <v>8864</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -11225,7 +11225,7 @@
         </is>
       </c>
       <c r="D84" t="n">
-        <v>10544.5</v>
+        <v>10544</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -11354,7 +11354,7 @@
         </is>
       </c>
       <c r="D85" t="n">
-        <v>10662.5</v>
+        <v>10662</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -11483,7 +11483,7 @@
         </is>
       </c>
       <c r="D86" t="n">
-        <v>10533.5</v>
+        <v>10533</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -11612,7 +11612,7 @@
         </is>
       </c>
       <c r="D87" t="n">
-        <v>7560.5</v>
+        <v>7560</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -11870,7 +11870,7 @@
         </is>
       </c>
       <c r="D89" t="n">
-        <v>10513.5</v>
+        <v>10513</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -11999,7 +11999,7 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>10661.5</v>
+        <v>10661</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -12128,7 +12128,7 @@
         </is>
       </c>
       <c r="D91" t="n">
-        <v>10907.5</v>
+        <v>10907</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -12257,7 +12257,7 @@
         </is>
       </c>
       <c r="D92" t="n">
-        <v>10466.5</v>
+        <v>10466</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -12386,7 +12386,7 @@
         </is>
       </c>
       <c r="D93" t="n">
-        <v>6578.5</v>
+        <v>6578</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -12515,7 +12515,7 @@
         </is>
       </c>
       <c r="D94" t="n">
-        <v>6423.5</v>
+        <v>6423</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -12644,7 +12644,7 @@
         </is>
       </c>
       <c r="D95" t="n">
-        <v>6423.5</v>
+        <v>6423</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -12773,7 +12773,7 @@
         </is>
       </c>
       <c r="D96" t="n">
-        <v>6423.5</v>
+        <v>6423</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -13031,7 +13031,7 @@
         </is>
       </c>
       <c r="D98" t="n">
-        <v>30902.5</v>
+        <v>30902</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -14321,7 +14321,7 @@
         </is>
       </c>
       <c r="D108" t="n">
-        <v>10482.5</v>
+        <v>10482</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -14450,7 +14450,7 @@
         </is>
       </c>
       <c r="D109" t="n">
-        <v>5393.5</v>
+        <v>5393</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -14837,7 +14837,7 @@
         </is>
       </c>
       <c r="D112" t="n">
-        <v>5778.5</v>
+        <v>5778</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -14966,7 +14966,7 @@
         </is>
       </c>
       <c r="D113" t="n">
-        <v>6705.5</v>
+        <v>6705</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -15353,7 +15353,7 @@
         </is>
       </c>
       <c r="D116" t="n">
-        <v>13457.5</v>
+        <v>13457</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -15482,7 +15482,7 @@
         </is>
       </c>
       <c r="D117" t="n">
-        <v>8222.5</v>
+        <v>8222</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -16256,7 +16256,7 @@
         </is>
       </c>
       <c r="D123" t="n">
-        <v>7179.5</v>
+        <v>7179</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -16385,7 +16385,7 @@
         </is>
       </c>
       <c r="D124" t="n">
-        <v>28737.5</v>
+        <v>28737</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -16514,7 +16514,7 @@
         </is>
       </c>
       <c r="D125" t="n">
-        <v>12774.5</v>
+        <v>12774</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -16772,7 +16772,7 @@
         </is>
       </c>
       <c r="D127" t="n">
-        <v>10279.5</v>
+        <v>10279</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -16901,7 +16901,7 @@
         </is>
       </c>
       <c r="D128" t="n">
-        <v>10789.5</v>
+        <v>10789</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -17159,7 +17159,7 @@
         </is>
       </c>
       <c r="D130" t="n">
-        <v>10063.5</v>
+        <v>10063</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -17675,7 +17675,7 @@
         </is>
       </c>
       <c r="D134" t="n">
-        <v>15200.5</v>
+        <v>15200</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -17804,7 +17804,7 @@
         </is>
       </c>
       <c r="D135" t="n">
-        <v>8155.5</v>
+        <v>8155</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -17933,7 +17933,7 @@
         </is>
       </c>
       <c r="D136" t="n">
-        <v>10482.5</v>
+        <v>10482</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -18062,7 +18062,7 @@
         </is>
       </c>
       <c r="D137" t="n">
-        <v>10482.5</v>
+        <v>10482</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -18191,7 +18191,7 @@
         </is>
       </c>
       <c r="D138" t="n">
-        <v>6423.5</v>
+        <v>6423</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -18449,7 +18449,7 @@
         </is>
       </c>
       <c r="D140" t="n">
-        <v>9142.5</v>
+        <v>9142</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -18578,7 +18578,7 @@
         </is>
       </c>
       <c r="D141" t="n">
-        <v>32653.5</v>
+        <v>32653</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -18707,7 +18707,7 @@
         </is>
       </c>
       <c r="D142" t="n">
-        <v>10065.5</v>
+        <v>10065</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -18965,7 +18965,7 @@
         </is>
       </c>
       <c r="D144" t="n">
-        <v>9338.5</v>
+        <v>9338</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -20255,7 +20255,7 @@
         </is>
       </c>
       <c r="D154" t="n">
-        <v>15555.5</v>
+        <v>15555</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -20513,7 +20513,7 @@
         </is>
       </c>
       <c r="D156" t="n">
-        <v>10477.5</v>
+        <v>10477</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -21029,7 +21029,7 @@
         </is>
       </c>
       <c r="D160" t="n">
-        <v>12993.5</v>
+        <v>12993</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -21287,7 +21287,7 @@
         </is>
       </c>
       <c r="D162" t="n">
-        <v>12993.5</v>
+        <v>12993</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -21674,7 +21674,7 @@
         </is>
       </c>
       <c r="D165" t="n">
-        <v>7939.5</v>
+        <v>7939</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -21803,7 +21803,7 @@
         </is>
       </c>
       <c r="D166" t="n">
-        <v>9437.5</v>
+        <v>9437</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -21932,7 +21932,7 @@
         </is>
       </c>
       <c r="D167" t="n">
-        <v>8046.5</v>
+        <v>8046</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -22190,7 +22190,7 @@
         </is>
       </c>
       <c r="D169" t="n">
-        <v>5244.5</v>
+        <v>5244</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -22706,7 +22706,7 @@
         </is>
       </c>
       <c r="D173" t="n">
-        <v>28081.5</v>
+        <v>28081</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -22964,7 +22964,7 @@
         </is>
       </c>
       <c r="D175" t="n">
-        <v>6593.5</v>
+        <v>6593</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -23351,7 +23351,7 @@
         </is>
       </c>
       <c r="D178" t="n">
-        <v>9510.5</v>
+        <v>9510</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -23480,7 +23480,7 @@
         </is>
       </c>
       <c r="D179" t="n">
-        <v>9146.5</v>
+        <v>9146</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -23609,7 +23609,7 @@
         </is>
       </c>
       <c r="D180" t="n">
-        <v>9874.5</v>
+        <v>9874</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -23867,7 +23867,7 @@
         </is>
       </c>
       <c r="D182" t="n">
-        <v>5535.5</v>
+        <v>5535</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -24125,7 +24125,7 @@
         </is>
       </c>
       <c r="D184" t="n">
-        <v>9692.5</v>
+        <v>9692</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -24254,7 +24254,7 @@
         </is>
       </c>
       <c r="D185" t="n">
-        <v>5460.5</v>
+        <v>5460</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -24641,7 +24641,7 @@
         </is>
       </c>
       <c r="D188" t="n">
-        <v>5096.5</v>
+        <v>5096</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -25157,7 +25157,7 @@
         </is>
       </c>
       <c r="D192" t="n">
-        <v>5391.5</v>
+        <v>5391</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -25415,7 +25415,7 @@
         </is>
       </c>
       <c r="D194" t="n">
-        <v>5563.5</v>
+        <v>5563</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -25544,7 +25544,7 @@
         </is>
       </c>
       <c r="D195" t="n">
-        <v>4340.5</v>
+        <v>4340</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -25673,7 +25673,7 @@
         </is>
       </c>
       <c r="D196" t="n">
-        <v>3765.5</v>
+        <v>3765</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -25802,7 +25802,7 @@
         </is>
       </c>
       <c r="D197" t="n">
-        <v>4495.5</v>
+        <v>4495</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -25931,7 +25931,7 @@
         </is>
       </c>
       <c r="D198" t="n">
-        <v>3299.5</v>
+        <v>3299</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -26060,7 +26060,7 @@
         </is>
       </c>
       <c r="D199" t="n">
-        <v>3305.5</v>
+        <v>3305</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -26705,7 +26705,7 @@
         </is>
       </c>
       <c r="D204" t="n">
-        <v>7047.5</v>
+        <v>7047</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -26834,7 +26834,7 @@
         </is>
       </c>
       <c r="D205" t="n">
-        <v>4898.5</v>
+        <v>4898</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -26963,7 +26963,7 @@
         </is>
       </c>
       <c r="D206" t="n">
-        <v>2751.5</v>
+        <v>2751</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -27221,7 +27221,7 @@
         </is>
       </c>
       <c r="D208" t="n">
-        <v>7680.5</v>
+        <v>7680</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -27350,7 +27350,7 @@
         </is>
       </c>
       <c r="D209" t="n">
-        <v>7057.5</v>
+        <v>7057</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -27737,7 +27737,7 @@
         </is>
       </c>
       <c r="D212" t="n">
-        <v>6952.5</v>
+        <v>6952</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -27866,7 +27866,7 @@
         </is>
       </c>
       <c r="D213" t="n">
-        <v>4630.5</v>
+        <v>4630</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -28253,7 +28253,7 @@
         </is>
       </c>
       <c r="D216" t="n">
-        <v>5663.5</v>
+        <v>5663</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -28382,7 +28382,7 @@
         </is>
       </c>
       <c r="D217" t="n">
-        <v>8203.5</v>
+        <v>8203</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -28511,7 +28511,7 @@
         </is>
       </c>
       <c r="D218" t="n">
-        <v>7857.5</v>
+        <v>7857</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -28640,7 +28640,7 @@
         </is>
       </c>
       <c r="D219" t="n">
-        <v>9133.5</v>
+        <v>9133</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -28898,7 +28898,7 @@
         </is>
       </c>
       <c r="D221" t="n">
-        <v>3737.5</v>
+        <v>3737</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -29027,7 +29027,7 @@
         </is>
       </c>
       <c r="D222" t="n">
-        <v>9926.5</v>
+        <v>9926</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -29156,7 +29156,7 @@
         </is>
       </c>
       <c r="D223" t="n">
-        <v>5780.5</v>
+        <v>5780</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -29414,7 +29414,7 @@
         </is>
       </c>
       <c r="D225" t="n">
-        <v>7297.5</v>
+        <v>7297</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -29543,7 +29543,7 @@
         </is>
       </c>
       <c r="D226" t="n">
-        <v>7549.5</v>
+        <v>7549</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -29672,7 +29672,7 @@
         </is>
       </c>
       <c r="D227" t="n">
-        <v>8186.5</v>
+        <v>8186</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -29801,7 +29801,7 @@
         </is>
       </c>
       <c r="D228" t="n">
-        <v>7655.5</v>
+        <v>7655</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -30059,7 +30059,7 @@
         </is>
       </c>
       <c r="D230" t="n">
-        <v>3358.5</v>
+        <v>3358</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -30188,7 +30188,7 @@
         </is>
       </c>
       <c r="D231" t="n">
-        <v>4526.5</v>
+        <v>4526</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -30446,7 +30446,7 @@
         </is>
       </c>
       <c r="D233" t="n">
-        <v>8177.5</v>
+        <v>8177</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -30704,7 +30704,7 @@
         </is>
       </c>
       <c r="D235" t="n">
-        <v>7802.5</v>
+        <v>7802</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -31349,7 +31349,7 @@
         </is>
       </c>
       <c r="D240" t="n">
-        <v>6748.5</v>
+        <v>6748</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -32123,7 +32123,7 @@
         </is>
       </c>
       <c r="D246" t="n">
-        <v>6680.5</v>
+        <v>6680</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -32252,7 +32252,7 @@
         </is>
       </c>
       <c r="D247" t="n">
-        <v>5603.5</v>
+        <v>5603</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -32381,7 +32381,7 @@
         </is>
       </c>
       <c r="D248" t="n">
-        <v>5668.5</v>
+        <v>5668</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -32510,7 +32510,7 @@
         </is>
       </c>
       <c r="D249" t="n">
-        <v>5662.5</v>
+        <v>5662</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -32768,7 +32768,7 @@
         </is>
       </c>
       <c r="D251" t="n">
-        <v>5452.5</v>
+        <v>5452</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -32897,7 +32897,7 @@
         </is>
       </c>
       <c r="D252" t="n">
-        <v>5562.5</v>
+        <v>5562</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -33671,7 +33671,7 @@
         </is>
       </c>
       <c r="D258" t="n">
-        <v>5267.5</v>
+        <v>5267</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -33800,7 +33800,7 @@
         </is>
       </c>
       <c r="D259" t="n">
-        <v>5464.5</v>
+        <v>5464</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -33929,7 +33929,7 @@
         </is>
       </c>
       <c r="D260" t="n">
-        <v>5938.5</v>
+        <v>5938</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -34058,7 +34058,7 @@
         </is>
       </c>
       <c r="D261" t="n">
-        <v>6033.5</v>
+        <v>6033</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -34187,7 +34187,7 @@
         </is>
       </c>
       <c r="D262" t="n">
-        <v>5385.5</v>
+        <v>5385</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -34445,7 +34445,7 @@
         </is>
       </c>
       <c r="D264" t="n">
-        <v>5456.5</v>
+        <v>5456</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -34703,7 +34703,7 @@
         </is>
       </c>
       <c r="D266" t="n">
-        <v>6918.5</v>
+        <v>6918</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -34961,7 +34961,7 @@
         </is>
       </c>
       <c r="D268" t="n">
-        <v>5389.5</v>
+        <v>5389</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -35090,7 +35090,7 @@
         </is>
       </c>
       <c r="D269" t="n">
-        <v>5603.5</v>
+        <v>5603</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -35348,7 +35348,7 @@
         </is>
       </c>
       <c r="D271" t="n">
-        <v>5450.5</v>
+        <v>5450</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -35606,7 +35606,7 @@
         </is>
       </c>
       <c r="D273" t="n">
-        <v>5746.5</v>
+        <v>5746</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -36380,7 +36380,7 @@
         </is>
       </c>
       <c r="D279" t="n">
-        <v>7227.5</v>
+        <v>7227</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -36638,7 +36638,7 @@
         </is>
       </c>
       <c r="D281" t="n">
-        <v>7295.5</v>
+        <v>7295</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -36767,7 +36767,7 @@
         </is>
       </c>
       <c r="D282" t="n">
-        <v>7107.5</v>
+        <v>7107</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -37154,7 +37154,7 @@
         </is>
       </c>
       <c r="D285" t="n">
-        <v>3697.5</v>
+        <v>3697</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -37283,7 +37283,7 @@
         </is>
       </c>
       <c r="D286" t="n">
-        <v>3967.5</v>
+        <v>3967</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -37541,7 +37541,7 @@
         </is>
       </c>
       <c r="D288" t="n">
-        <v>3747.5</v>
+        <v>3747</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -37670,7 +37670,7 @@
         </is>
       </c>
       <c r="D289" t="n">
-        <v>3760.5</v>
+        <v>3760</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -37799,7 +37799,7 @@
         </is>
       </c>
       <c r="D290" t="n">
-        <v>3923.5</v>
+        <v>3923</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -37928,7 +37928,7 @@
         </is>
       </c>
       <c r="D291" t="n">
-        <v>3840.5</v>
+        <v>3840</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -38186,7 +38186,7 @@
         </is>
       </c>
       <c r="D293" t="n">
-        <v>4959.5</v>
+        <v>4959</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -38573,7 +38573,7 @@
         </is>
       </c>
       <c r="D296" t="n">
-        <v>6512.5</v>
+        <v>6512</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -38702,7 +38702,7 @@
         </is>
       </c>
       <c r="D297" t="n">
-        <v>5534.5</v>
+        <v>5534</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -39089,7 +39089,7 @@
         </is>
       </c>
       <c r="D300" t="n">
-        <v>2742.5</v>
+        <v>2742</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -39476,7 +39476,7 @@
         </is>
       </c>
       <c r="D303" t="n">
-        <v>6035.5</v>
+        <v>6035</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -39605,7 +39605,7 @@
         </is>
       </c>
       <c r="D304" t="n">
-        <v>6677.5</v>
+        <v>6677</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -39734,7 +39734,7 @@
         </is>
       </c>
       <c r="D305" t="n">
-        <v>6838.5</v>
+        <v>6838</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -39992,7 +39992,7 @@
         </is>
       </c>
       <c r="D307" t="n">
-        <v>6610.5</v>
+        <v>6610</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -40250,7 +40250,7 @@
         </is>
       </c>
       <c r="D309" t="n">
-        <v>7455.5</v>
+        <v>7455</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -40637,7 +40637,7 @@
         </is>
       </c>
       <c r="D312" t="n">
-        <v>10654.5</v>
+        <v>10654</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -40766,7 +40766,7 @@
         </is>
       </c>
       <c r="D313" t="n">
-        <v>10740.5</v>
+        <v>10740</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -40895,7 +40895,7 @@
         </is>
       </c>
       <c r="D314" t="n">
-        <v>10654.5</v>
+        <v>10654</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -41024,7 +41024,7 @@
         </is>
       </c>
       <c r="D315" t="n">
-        <v>10654.5</v>
+        <v>10654</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -41153,7 +41153,7 @@
         </is>
       </c>
       <c r="D316" t="n">
-        <v>7055.5</v>
+        <v>7055</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -41411,7 +41411,7 @@
         </is>
       </c>
       <c r="D318" t="n">
-        <v>6615.5</v>
+        <v>6615</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -41798,7 +41798,7 @@
         </is>
       </c>
       <c r="D321" t="n">
-        <v>6303.5</v>
+        <v>6303</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -42056,7 +42056,7 @@
         </is>
       </c>
       <c r="D323" t="n">
-        <v>6622.5</v>
+        <v>6622</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -42314,7 +42314,7 @@
         </is>
       </c>
       <c r="D325" t="n">
-        <v>2151.5</v>
+        <v>2151</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -42572,7 +42572,7 @@
         </is>
       </c>
       <c r="D327" t="n">
-        <v>6054.5</v>
+        <v>6054</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -42959,7 +42959,7 @@
         </is>
       </c>
       <c r="D330" t="n">
-        <v>6841.5</v>
+        <v>6841</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -43088,7 +43088,7 @@
         </is>
       </c>
       <c r="D331" t="n">
-        <v>6743.5</v>
+        <v>6743</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -43604,7 +43604,7 @@
         </is>
       </c>
       <c r="D335" t="n">
-        <v>10056.5</v>
+        <v>10056</v>
       </c>
       <c r="E335" t="inlineStr">
         <is>
@@ -43862,7 +43862,7 @@
         </is>
       </c>
       <c r="D337" t="n">
-        <v>10564.5</v>
+        <v>10564</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -44507,7 +44507,7 @@
         </is>
       </c>
       <c r="D342" t="n">
-        <v>8064.5</v>
+        <v>8064</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -44894,7 +44894,7 @@
         </is>
       </c>
       <c r="D345" t="n">
-        <v>7911.5</v>
+        <v>7911</v>
       </c>
       <c r="E345" t="inlineStr">
         <is>
@@ -45023,7 +45023,7 @@
         </is>
       </c>
       <c r="D346" t="n">
-        <v>8084.5</v>
+        <v>8084</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -45281,7 +45281,7 @@
         </is>
       </c>
       <c r="D348" t="n">
-        <v>7904.5</v>
+        <v>7904</v>
       </c>
       <c r="E348" t="inlineStr">
         <is>
@@ -45410,7 +45410,7 @@
         </is>
       </c>
       <c r="D349" t="n">
-        <v>8183.5</v>
+        <v>8183</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -45668,7 +45668,7 @@
         </is>
       </c>
       <c r="D351" t="n">
-        <v>5534.5</v>
+        <v>5534</v>
       </c>
       <c r="E351" t="inlineStr">
         <is>
@@ -45797,7 +45797,7 @@
         </is>
       </c>
       <c r="D352" t="n">
-        <v>5134.5</v>
+        <v>5134</v>
       </c>
       <c r="E352" t="inlineStr">
         <is>
@@ -46055,7 +46055,7 @@
         </is>
       </c>
       <c r="D354" t="n">
-        <v>6144.5</v>
+        <v>6144</v>
       </c>
       <c r="E354" t="inlineStr">
         <is>
@@ -46184,7 +46184,7 @@
         </is>
       </c>
       <c r="D355" t="n">
-        <v>6371.5</v>
+        <v>6371</v>
       </c>
       <c r="E355" t="inlineStr">
         <is>
@@ -46313,7 +46313,7 @@
         </is>
       </c>
       <c r="D356" t="n">
-        <v>5534.5</v>
+        <v>5534</v>
       </c>
       <c r="E356" t="inlineStr">
         <is>
@@ -46442,7 +46442,7 @@
         </is>
       </c>
       <c r="D357" t="n">
-        <v>4611.5</v>
+        <v>4611</v>
       </c>
       <c r="E357" t="inlineStr">
         <is>
@@ -46700,7 +46700,7 @@
         </is>
       </c>
       <c r="D359" t="n">
-        <v>7029.5</v>
+        <v>7029</v>
       </c>
       <c r="E359" t="inlineStr">
         <is>
@@ -47216,7 +47216,7 @@
         </is>
       </c>
       <c r="D363" t="n">
-        <v>5180.5</v>
+        <v>5180</v>
       </c>
       <c r="E363" t="inlineStr">
         <is>
@@ -47345,7 +47345,7 @@
         </is>
       </c>
       <c r="D364" t="n">
-        <v>5544.5</v>
+        <v>5544</v>
       </c>
       <c r="E364" t="inlineStr">
         <is>
@@ -47474,7 +47474,7 @@
         </is>
       </c>
       <c r="D365" t="n">
-        <v>5213.5</v>
+        <v>5213</v>
       </c>
       <c r="E365" t="inlineStr">
         <is>
@@ -47732,7 +47732,7 @@
         </is>
       </c>
       <c r="D367" t="n">
-        <v>5140.5</v>
+        <v>5140</v>
       </c>
       <c r="E367" t="inlineStr">
         <is>
@@ -47861,7 +47861,7 @@
         </is>
       </c>
       <c r="D368" t="n">
-        <v>7814.5</v>
+        <v>7814</v>
       </c>
       <c r="E368" t="inlineStr">
         <is>
@@ -48248,7 +48248,7 @@
         </is>
       </c>
       <c r="D371" t="n">
-        <v>4336.5</v>
+        <v>4336</v>
       </c>
       <c r="E371" t="inlineStr">
         <is>
@@ -48377,7 +48377,7 @@
         </is>
       </c>
       <c r="D372" t="n">
-        <v>4330.5</v>
+        <v>4330</v>
       </c>
       <c r="E372" t="inlineStr">
         <is>
@@ -48506,7 +48506,7 @@
         </is>
       </c>
       <c r="D373" t="n">
-        <v>4896.5</v>
+        <v>4896</v>
       </c>
       <c r="E373" t="inlineStr">
         <is>
@@ -48635,7 +48635,7 @@
         </is>
       </c>
       <c r="D374" t="n">
-        <v>5079.5</v>
+        <v>5079</v>
       </c>
       <c r="E374" t="inlineStr">
         <is>
@@ -48764,7 +48764,7 @@
         </is>
       </c>
       <c r="D375" t="n">
-        <v>5081.5</v>
+        <v>5081</v>
       </c>
       <c r="E375" t="inlineStr">
         <is>
@@ -49151,7 +49151,7 @@
         </is>
       </c>
       <c r="D378" t="n">
-        <v>7134.5</v>
+        <v>7134</v>
       </c>
       <c r="E378" t="inlineStr">
         <is>
@@ -49538,7 +49538,7 @@
         </is>
       </c>
       <c r="D381" t="n">
-        <v>5131.5</v>
+        <v>5131</v>
       </c>
       <c r="E381" t="inlineStr">
         <is>
@@ -49667,7 +49667,7 @@
         </is>
       </c>
       <c r="D382" t="n">
-        <v>5835.5</v>
+        <v>5835</v>
       </c>
       <c r="E382" t="inlineStr">
         <is>
@@ -49796,7 +49796,7 @@
         </is>
       </c>
       <c r="D383" t="n">
-        <v>8273.5</v>
+        <v>8273</v>
       </c>
       <c r="E383" t="inlineStr">
         <is>
@@ -50312,7 +50312,7 @@
         </is>
       </c>
       <c r="D387" t="n">
-        <v>3417.5</v>
+        <v>3417</v>
       </c>
       <c r="E387" t="inlineStr">
         <is>
@@ -50699,7 +50699,7 @@
         </is>
       </c>
       <c r="D390" t="n">
-        <v>8014.5</v>
+        <v>8014</v>
       </c>
       <c r="E390" t="inlineStr">
         <is>
@@ -50957,7 +50957,7 @@
         </is>
       </c>
       <c r="D392" t="n">
-        <v>8658.5</v>
+        <v>8658</v>
       </c>
       <c r="E392" t="inlineStr">
         <is>
@@ -51215,7 +51215,7 @@
         </is>
       </c>
       <c r="D394" t="n">
-        <v>5589.5</v>
+        <v>5589</v>
       </c>
       <c r="E394" t="inlineStr">
         <is>
@@ -51473,7 +51473,7 @@
         </is>
       </c>
       <c r="D396" t="n">
-        <v>6906.5</v>
+        <v>6906</v>
       </c>
       <c r="E396" t="inlineStr">
         <is>
@@ -51731,7 +51731,7 @@
         </is>
       </c>
       <c r="D398" t="n">
-        <v>5442.5</v>
+        <v>5442</v>
       </c>
       <c r="E398" t="inlineStr">
         <is>
@@ -52118,7 +52118,7 @@
         </is>
       </c>
       <c r="D401" t="n">
-        <v>5270.5</v>
+        <v>5270</v>
       </c>
       <c r="E401" t="inlineStr">
         <is>
@@ -52247,7 +52247,7 @@
         </is>
       </c>
       <c r="D402" t="n">
-        <v>4849.5</v>
+        <v>4849</v>
       </c>
       <c r="E402" t="inlineStr">
         <is>
@@ -52505,7 +52505,7 @@
         </is>
       </c>
       <c r="D404" t="n">
-        <v>6811.5</v>
+        <v>6811</v>
       </c>
       <c r="E404" t="inlineStr">
         <is>
@@ -52634,7 +52634,7 @@
         </is>
       </c>
       <c r="D405" t="n">
-        <v>6818.5</v>
+        <v>6818</v>
       </c>
       <c r="E405" t="inlineStr">
         <is>
@@ -52892,7 +52892,7 @@
         </is>
       </c>
       <c r="D407" t="n">
-        <v>4110.5</v>
+        <v>4110</v>
       </c>
       <c r="E407" t="inlineStr">
         <is>
@@ -53537,7 +53537,7 @@
         </is>
       </c>
       <c r="D412" t="n">
-        <v>6985.5</v>
+        <v>6985</v>
       </c>
       <c r="E412" t="inlineStr">
         <is>
@@ -53666,7 +53666,7 @@
         </is>
       </c>
       <c r="D413" t="n">
-        <v>6727.5</v>
+        <v>6727</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -53924,7 +53924,7 @@
         </is>
       </c>
       <c r="D415" t="n">
-        <v>7071.5</v>
+        <v>7071</v>
       </c>
       <c r="E415" t="inlineStr">
         <is>
@@ -54182,7 +54182,7 @@
         </is>
       </c>
       <c r="D417" t="n">
-        <v>3648.5</v>
+        <v>3648</v>
       </c>
       <c r="E417" t="inlineStr">
         <is>
@@ -54311,7 +54311,7 @@
         </is>
       </c>
       <c r="D418" t="n">
-        <v>5532.5</v>
+        <v>5532</v>
       </c>
       <c r="E418" t="inlineStr">
         <is>
@@ -54698,7 +54698,7 @@
         </is>
       </c>
       <c r="D421" t="n">
-        <v>5667.5</v>
+        <v>5667</v>
       </c>
       <c r="E421" t="inlineStr">
         <is>
@@ -55085,7 +55085,7 @@
         </is>
       </c>
       <c r="D424" t="n">
-        <v>5329.5</v>
+        <v>5329</v>
       </c>
       <c r="E424" t="inlineStr">
         <is>
@@ -55343,7 +55343,7 @@
         </is>
       </c>
       <c r="D426" t="n">
-        <v>6544.5</v>
+        <v>6544</v>
       </c>
       <c r="E426" t="inlineStr">
         <is>
@@ -55730,7 +55730,7 @@
         </is>
       </c>
       <c r="D429" t="n">
-        <v>3473.5</v>
+        <v>3473</v>
       </c>
       <c r="E429" t="inlineStr">
         <is>
@@ -55988,7 +55988,7 @@
         </is>
       </c>
       <c r="D431" t="n">
-        <v>9391.5</v>
+        <v>9391</v>
       </c>
       <c r="E431" t="inlineStr">
         <is>
@@ -56117,7 +56117,7 @@
         </is>
       </c>
       <c r="D432" t="n">
-        <v>9290.5</v>
+        <v>9290</v>
       </c>
       <c r="E432" t="inlineStr">
         <is>
@@ -56375,7 +56375,7 @@
         </is>
       </c>
       <c r="D434" t="n">
-        <v>4664.5</v>
+        <v>4664</v>
       </c>
       <c r="E434" t="inlineStr">
         <is>
@@ -56504,7 +56504,7 @@
         </is>
       </c>
       <c r="D435" t="n">
-        <v>4745.5</v>
+        <v>4745</v>
       </c>
       <c r="E435" t="inlineStr">
         <is>
@@ -56633,7 +56633,7 @@
         </is>
       </c>
       <c r="D436" t="n">
-        <v>5392.5</v>
+        <v>5392</v>
       </c>
       <c r="E436" t="inlineStr">
         <is>
@@ -57278,7 +57278,7 @@
         </is>
       </c>
       <c r="D441" t="n">
-        <v>6305.5</v>
+        <v>6305</v>
       </c>
       <c r="E441" t="inlineStr">
         <is>
@@ -57407,7 +57407,7 @@
         </is>
       </c>
       <c r="D442" t="n">
-        <v>6044.5</v>
+        <v>6044</v>
       </c>
       <c r="E442" t="inlineStr">
         <is>
@@ -57536,7 +57536,7 @@
         </is>
       </c>
       <c r="D443" t="n">
-        <v>6298.5</v>
+        <v>6298</v>
       </c>
       <c r="E443" t="inlineStr">
         <is>
@@ -57665,7 +57665,7 @@
         </is>
       </c>
       <c r="D444" t="n">
-        <v>6777.5</v>
+        <v>6777</v>
       </c>
       <c r="E444" t="inlineStr">
         <is>
@@ -57794,7 +57794,7 @@
         </is>
       </c>
       <c r="D445" t="n">
-        <v>3667.5</v>
+        <v>3667</v>
       </c>
       <c r="E445" t="inlineStr">
         <is>
@@ -57923,7 +57923,7 @@
         </is>
       </c>
       <c r="D446" t="n">
-        <v>3666.5</v>
+        <v>3666</v>
       </c>
       <c r="E446" t="inlineStr">
         <is>
@@ -58052,7 +58052,7 @@
         </is>
       </c>
       <c r="D447" t="n">
-        <v>4110.5</v>
+        <v>4110</v>
       </c>
       <c r="E447" t="inlineStr">
         <is>
@@ -58181,7 +58181,7 @@
         </is>
       </c>
       <c r="D448" t="n">
-        <v>5183.5</v>
+        <v>5183</v>
       </c>
       <c r="E448" t="inlineStr">
         <is>
@@ -58310,7 +58310,7 @@
         </is>
       </c>
       <c r="D449" t="n">
-        <v>5456.5</v>
+        <v>5456</v>
       </c>
       <c r="E449" t="inlineStr">
         <is>
@@ -58439,7 +58439,7 @@
         </is>
       </c>
       <c r="D450" t="n">
-        <v>4254.5</v>
+        <v>4254</v>
       </c>
       <c r="E450" t="inlineStr">
         <is>
@@ -58568,7 +58568,7 @@
         </is>
       </c>
       <c r="D451" t="n">
-        <v>4015.5</v>
+        <v>4015</v>
       </c>
       <c r="E451" t="inlineStr">
         <is>
@@ -58697,7 +58697,7 @@
         </is>
       </c>
       <c r="D452" t="n">
-        <v>3985.5</v>
+        <v>3985</v>
       </c>
       <c r="E452" t="inlineStr">
         <is>
@@ -58826,7 +58826,7 @@
         </is>
       </c>
       <c r="D453" t="n">
-        <v>4384.5</v>
+        <v>4384</v>
       </c>
       <c r="E453" t="inlineStr">
         <is>
@@ -58955,7 +58955,7 @@
         </is>
       </c>
       <c r="D454" t="n">
-        <v>4037.5</v>
+        <v>4037</v>
       </c>
       <c r="E454" t="inlineStr">
         <is>
@@ -59213,7 +59213,7 @@
         </is>
       </c>
       <c r="D456" t="n">
-        <v>5388.5</v>
+        <v>5388</v>
       </c>
       <c r="E456" t="inlineStr">
         <is>
@@ -59342,7 +59342,7 @@
         </is>
       </c>
       <c r="D457" t="n">
-        <v>5713.5</v>
+        <v>5713</v>
       </c>
       <c r="E457" t="inlineStr">
         <is>
@@ -59471,7 +59471,7 @@
         </is>
       </c>
       <c r="D458" t="n">
-        <v>5443.5</v>
+        <v>5443</v>
       </c>
       <c r="E458" t="inlineStr">
         <is>
@@ -59858,7 +59858,7 @@
         </is>
       </c>
       <c r="D461" t="n">
-        <v>3803.5</v>
+        <v>3803</v>
       </c>
       <c r="E461" t="inlineStr">
         <is>
@@ -59987,7 +59987,7 @@
         </is>
       </c>
       <c r="D462" t="n">
-        <v>1168.5</v>
+        <v>1168</v>
       </c>
       <c r="E462" t="inlineStr">
         <is>
@@ -60374,7 +60374,7 @@
         </is>
       </c>
       <c r="D465" t="n">
-        <v>5648.5</v>
+        <v>5648</v>
       </c>
       <c r="E465" t="inlineStr">
         <is>
@@ -60632,7 +60632,7 @@
         </is>
       </c>
       <c r="D467" t="n">
-        <v>6779.5</v>
+        <v>6779</v>
       </c>
       <c r="E467" t="inlineStr">
         <is>
@@ -60761,7 +60761,7 @@
         </is>
       </c>
       <c r="D468" t="n">
-        <v>5535.5</v>
+        <v>5535</v>
       </c>
       <c r="E468" t="inlineStr">
         <is>
@@ -60890,7 +60890,7 @@
         </is>
       </c>
       <c r="D469" t="n">
-        <v>5726.5</v>
+        <v>5726</v>
       </c>
       <c r="E469" t="inlineStr">
         <is>
@@ -61406,7 +61406,7 @@
         </is>
       </c>
       <c r="D473" t="n">
-        <v>4097.5</v>
+        <v>4097</v>
       </c>
       <c r="E473" t="inlineStr">
         <is>
@@ -61664,7 +61664,7 @@
         </is>
       </c>
       <c r="D475" t="n">
-        <v>5813.5</v>
+        <v>5813</v>
       </c>
       <c r="E475" t="inlineStr">
         <is>
@@ -61793,7 +61793,7 @@
         </is>
       </c>
       <c r="D476" t="n">
-        <v>4946.5</v>
+        <v>4946</v>
       </c>
       <c r="E476" t="inlineStr">
         <is>
@@ -62309,7 +62309,7 @@
         </is>
       </c>
       <c r="D480" t="n">
-        <v>3833.5</v>
+        <v>3833</v>
       </c>
       <c r="E480" t="inlineStr">
         <is>
@@ -62438,7 +62438,7 @@
         </is>
       </c>
       <c r="D481" t="n">
-        <v>5247.5</v>
+        <v>5247</v>
       </c>
       <c r="E481" t="inlineStr">
         <is>
@@ -62567,7 +62567,7 @@
         </is>
       </c>
       <c r="D482" t="n">
-        <v>7877.5</v>
+        <v>7877</v>
       </c>
       <c r="E482" t="inlineStr">
         <is>
@@ -62954,7 +62954,7 @@
         </is>
       </c>
       <c r="D485" t="n">
-        <v>4616.5</v>
+        <v>4616</v>
       </c>
       <c r="E485" t="inlineStr">
         <is>
@@ -63083,7 +63083,7 @@
         </is>
       </c>
       <c r="D486" t="n">
-        <v>5443.5</v>
+        <v>5443</v>
       </c>
       <c r="E486" t="inlineStr">
         <is>
@@ -63212,7 +63212,7 @@
         </is>
       </c>
       <c r="D487" t="n">
-        <v>3144.5</v>
+        <v>3144</v>
       </c>
       <c r="E487" t="inlineStr">
         <is>
@@ -63470,7 +63470,7 @@
         </is>
       </c>
       <c r="D489" t="n">
-        <v>5962.5</v>
+        <v>5962</v>
       </c>
       <c r="E489" t="inlineStr">
         <is>
@@ -63599,7 +63599,7 @@
         </is>
       </c>
       <c r="D490" t="n">
-        <v>5148.5</v>
+        <v>5148</v>
       </c>
       <c r="E490" t="inlineStr">
         <is>
@@ -63728,7 +63728,7 @@
         </is>
       </c>
       <c r="D491" t="n">
-        <v>5785.5</v>
+        <v>5785</v>
       </c>
       <c r="E491" t="inlineStr">
         <is>

</xml_diff>